<commit_message>
Adjust costs where relying on US data
</commit_message>
<xml_diff>
--- a/InputData/bldgs/CpUDSC/Cost per Unit Dist Solar Cap.xlsx
+++ b/InputData/bldgs/CpUDSC/Cost per Unit Dist Solar Cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\bldgs\CpUDSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-eu\InputData\bldgs\CpUDSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F11FE36-41F2-4CC9-B172-CB91A4E38E2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F77EBA-C9ED-44BC-B29C-F83B04943CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="1260" windowWidth="21600" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>CpUDSC Cost per Unit Distributed Solar Capacity</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Distributed Solar Total Cap Cost</t>
+  </si>
+  <si>
+    <t>We adjust for the ratio of EU:US solar PV power plants (see file scaling factors).</t>
+  </si>
+  <si>
+    <t>Scaling factor</t>
   </si>
 </sst>
 </file>
@@ -491,6 +497,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="12"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -509,14 +523,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="12"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -868,21 +874,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -890,119 +898,132 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B12" s="2">
         <v>2015</v>
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32">
+        <v>0.91218637586370321</v>
       </c>
     </row>
   </sheetData>
@@ -1021,19 +1042,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.85899999999999999</v>
       </c>
@@ -1041,10 +1062,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
     </row>
   </sheetData>
@@ -1059,18 +1080,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="33.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="C3">
         <v>2018</v>
       </c>
@@ -1171,7 +1192,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1278,7 +1299,7 @@
         <v>602.42092125560248</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -1382,7 +1403,7 @@
         <v>857.6570833640435</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -1486,7 +1507,7 @@
         <v>1124.6145820191289</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1590,7 +1611,7 @@
         <v>602.42092125560248</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1694,7 +1715,7 @@
         <v>857.6570833640435</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -1798,7 +1819,7 @@
         <v>1124.6145820191289</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -1902,7 +1923,7 @@
         <v>602.42092125560248</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>27</v>
       </c>
@@ -2006,7 +2027,7 @@
         <v>857.6570833640435</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -2110,7 +2131,7 @@
         <v>1124.6145820191289</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>29</v>
       </c>
@@ -2214,7 +2235,7 @@
         <v>602.42092125560248</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>30</v>
       </c>
@@ -2318,7 +2339,7 @@
         <v>857.6570833640435</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -2422,7 +2443,7 @@
         <v>1124.6145820191289</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -2526,7 +2547,7 @@
         <v>602.42092125560248</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -2630,7 +2651,7 @@
         <v>857.6570833640435</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -2734,45 +2755,45 @@
         <v>1124.6145820191289</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A21" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2791,66 +2812,66 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="10">
         <v>0.63</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="10">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="10">
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="11">
         <f>AVERAGE(B4:B5)</f>
         <v>0.59499999999999997</v>
       </c>
@@ -2867,308 +2888,310 @@
   </sheetPr>
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A2,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>3255232.9117624536</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A2,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>2969379.1123728426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A3,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>3078322.0757814161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A3,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>2808003.4580482822</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A4,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>2901411.2398003791</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A4,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>2646627.8037237218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2022</v>
       </c>
       <c r="B5" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A5,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>2724500.4038193417</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A5,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>2485252.1493991613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2023</v>
       </c>
       <c r="B6" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A6,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>2547589.5678383047</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A6,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>2323876.4950746009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A7,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>2370678.7318572667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A7,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>2162500.84075004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A8,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>2193767.8958762302</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A8,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>2001125.1864254803</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A9,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>2016857.059895193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A9,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1839749.5321009199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A10,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1839946.223914156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A10,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1678373.8777763597</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A11,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1663035.387933119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A11,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1516998.2234517995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2029</v>
       </c>
       <c r="B12" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A12,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1486124.551952082</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A12,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1355622.5691272393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A13,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1309213.7159710464</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A13,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1194246.9148026805</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2031</v>
       </c>
       <c r="B14" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A14,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1293674.8627315189</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A14,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1180072.584581038</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2032</v>
       </c>
       <c r="B15" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A15,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1278136.009491991</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A15,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1165898.254359395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2033</v>
       </c>
       <c r="B16" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A16,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1262597.1562524636</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A16,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1151723.9241377525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2034</v>
       </c>
       <c r="B17" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A17,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1247058.3030129359</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A17,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1137549.5939161098</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2035</v>
       </c>
       <c r="B18" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A18,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1231519.449773408</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A18,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1123375.263694467</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2036</v>
       </c>
       <c r="B19" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A19,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1215980.5965338806</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A19,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1109200.9334728245</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2037</v>
       </c>
       <c r="B20" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A20,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1200441.7432943531</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A20,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1095026.603251182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2038</v>
       </c>
       <c r="B21" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A21,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1184902.8900548255</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A21,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1080852.2730295393</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2039</v>
       </c>
       <c r="B22" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A22,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1169364.0368152976</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A22,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1066677.9428078963</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A23,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1153825.1835757701</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A23,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1052503.6125862538</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2041</v>
       </c>
       <c r="B24" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A24,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1138286.3303362424</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A24,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1038329.282364611</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2042</v>
       </c>
       <c r="B25" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A25,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1122747.4770967148</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A25,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1024154.9521429684</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2043</v>
       </c>
       <c r="B26" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A26,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1107208.6238571871</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A26,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>1009980.6219213257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2044</v>
       </c>
       <c r="B27" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A27,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1091669.7706176594</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A27,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>995806.29169968294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2045</v>
       </c>
       <c r="B28" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A28,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1076130.9173781318</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A28,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>981631.9614780402</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2046</v>
       </c>
       <c r="B29" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A29,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1060592.0641386043</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A29,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>967457.6312563977</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2047</v>
       </c>
       <c r="B30" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A30,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1045053.2108990765</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A30,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>953283.30103475496</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2048</v>
       </c>
       <c r="B31" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A31,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1029514.3576595489</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A31,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>939108.97081311222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2049</v>
       </c>
       <c r="B32" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A32,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>1013975.5044200213</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A32,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>924934.64059146959</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2050</v>
       </c>
       <c r="B33" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A33,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
-        <v>998436.65118049306</v>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A33,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3*About!$B$32</f>
+        <v>910760.31036982639</v>
       </c>
     </row>
   </sheetData>
@@ -3183,308 +3206,310 @@
   </sheetPr>
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B2</f>
-        <v>1936863.5824986598</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B2*About!$B$32</f>
+        <v>1611633.166793054</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B3</f>
-        <v>1831601.6350899425</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B3*About!$B$32</f>
+        <v>1524046.3861968361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B4</f>
-        <v>1726339.6876812256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B4*About!$B$32</f>
+        <v>1436459.6056006181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2022</v>
       </c>
       <c r="B5" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B5</f>
-        <v>1621077.7402725082</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B5*About!$B$32</f>
+        <v>1348872.8250044002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2023</v>
       </c>
       <c r="B6" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B6</f>
-        <v>1515815.7928637911</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B6*About!$B$32</f>
+        <v>1261286.0444081824</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B7</f>
-        <v>1410553.8454550738</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B7*About!$B$32</f>
+        <v>1173699.2638119641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B8</f>
-        <v>1305291.8980463569</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B8*About!$B$32</f>
+        <v>1086112.4832157467</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B9</f>
-        <v>1200029.9506376397</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B9*About!$B$32</f>
+        <v>998525.70261952863</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B10</f>
-        <v>1094768.0032289228</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B10*About!$B$32</f>
+        <v>910938.92202331079</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B11</f>
-        <v>989506.05582020571</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B11*About!$B$32</f>
+        <v>823352.14142709307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2029</v>
       </c>
       <c r="B12" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B12</f>
-        <v>884244.10841148871</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B12*About!$B$32</f>
+        <v>735765.36083087523</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B13</f>
-        <v>778982.16100277251</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B13*About!$B$32</f>
+        <v>648178.58023465821</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2031</v>
       </c>
       <c r="B14" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B14</f>
-        <v>769736.54332525376</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B14*About!$B$32</f>
+        <v>640485.44984012877</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2032</v>
       </c>
       <c r="B15" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B15</f>
-        <v>760490.92564773466</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B15*About!$B$32</f>
+        <v>632792.3194455991</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2033</v>
       </c>
       <c r="B16" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B16</f>
-        <v>751245.3079702158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B16*About!$B$32</f>
+        <v>625099.18905106978</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2034</v>
       </c>
       <c r="B17" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B17</f>
-        <v>741999.69029269682</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B17*About!$B$32</f>
+        <v>617406.05865654023</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2035</v>
       </c>
       <c r="B18" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B18</f>
-        <v>732754.07261517772</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B18*About!$B$32</f>
+        <v>609712.92826201068</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2036</v>
       </c>
       <c r="B19" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B19</f>
-        <v>723508.45493765885</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B19*About!$B$32</f>
+        <v>602019.79786748136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2037</v>
       </c>
       <c r="B20" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B20</f>
-        <v>714262.83726014011</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B20*About!$B$32</f>
+        <v>594326.66747295193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2038</v>
       </c>
       <c r="B21" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B21</f>
-        <v>705017.21958262112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B21*About!$B$32</f>
+        <v>586633.53707842238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2039</v>
       </c>
       <c r="B22" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B22</f>
-        <v>695771.60190510203</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B22*About!$B$32</f>
+        <v>578940.40668389283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B23</f>
-        <v>686525.98422758316</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B23*About!$B$32</f>
+        <v>571247.27628936339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2041</v>
       </c>
       <c r="B24" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B24</f>
-        <v>677280.36655006418</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B24*About!$B$32</f>
+        <v>563554.14589483384</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2042</v>
       </c>
       <c r="B25" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B25</f>
-        <v>668034.74887254531</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B25*About!$B$32</f>
+        <v>555861.01550030441</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2043</v>
       </c>
       <c r="B26" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B26</f>
-        <v>658789.13119502633</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B26*About!$B$32</f>
+        <v>548167.88510577497</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2044</v>
       </c>
       <c r="B27" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B27</f>
-        <v>649543.51351750735</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B27*About!$B$32</f>
+        <v>540474.75471124542</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2045</v>
       </c>
       <c r="B28" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B28</f>
-        <v>640297.89583998837</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B28*About!$B$32</f>
+        <v>532781.62431671587</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2046</v>
       </c>
       <c r="B29" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B29</f>
-        <v>631052.27816246951</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B29*About!$B$32</f>
+        <v>525088.49392218655</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2047</v>
       </c>
       <c r="B30" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B30</f>
-        <v>621806.66048495052</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B30*About!$B$32</f>
+        <v>517395.36352765694</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2048</v>
       </c>
       <c r="B31" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B31</f>
-        <v>612561.04280743154</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B31*About!$B$32</f>
+        <v>509702.23313312751</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2049</v>
       </c>
       <c r="B32" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B32</f>
-        <v>603315.42512991268</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B32*About!$B$32</f>
+        <v>502009.10273859801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2050</v>
       </c>
       <c r="B33" s="7">
-        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B33</f>
-        <v>594069.80745239335</v>
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B33*About!$B$32</f>
+        <v>494315.97234406823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>